<commit_message>
se actualiza la cotizacion para evitar sobre paso
</commit_message>
<xml_diff>
--- a/config/cotizacion.xlsx
+++ b/config/cotizacion.xlsx
@@ -346,9 +346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>849240</xdr:colOff>
+      <xdr:colOff>848880</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>105840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -362,7 +362,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="197280" y="10080"/>
-          <a:ext cx="3407760" cy="1910880"/>
+          <a:ext cx="4131360" cy="1910520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -380,12 +380,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S16" activeCellId="0" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -995,7 +995,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.3" bottom="0.3" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="93" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>